<commit_message>
Remove the Person sheet since we need to populate Person based on the demoBookingCount. Add more values to PersonRace, BondType and make the PersonAgeID the same values as AgeInYears.
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/AnalyticsCodeTables.xlsx
+++ b/booking-jail/r-load/AnalyticsCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-29360" yWindow="2960" windowWidth="18200" windowHeight="12080" tabRatio="663" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="663" firstSheet="7" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="YesNo" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,6 @@
     <sheet name="Jurisdiction" sheetId="20" r:id="rId13"/>
     <sheet name="PopulationType" sheetId="22" r:id="rId14"/>
     <sheet name="PretrialStatus" sheetId="23" r:id="rId15"/>
-    <sheet name="Person" sheetId="24" r:id="rId16"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="95">
   <si>
     <t>Yes</t>
   </si>
@@ -312,28 +311,13 @@
     <t>AgeRangeSort</t>
   </si>
   <si>
-    <t>PersonID</t>
-  </si>
-  <si>
-    <t>StagingPersonUniqueIdentifier</t>
-  </si>
-  <si>
-    <t>I0000001</t>
-  </si>
-  <si>
-    <t>I0000002</t>
-  </si>
-  <si>
-    <t>I0000003</t>
-  </si>
-  <si>
-    <t>I0000004</t>
-  </si>
-  <si>
-    <t>I0000005</t>
-  </si>
-  <si>
-    <t>I0000006</t>
+    <t>Hispanic</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>Deposit</t>
   </si>
 </sst>
 </file>
@@ -382,8 +366,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -399,17 +385,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1096,7 +1084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1151,85 +1139,6 @@
       </c>
       <c r="B6" t="s">
         <v>83</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1244,10 +1153,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1290,22 +1199,31 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1375,7 +1293,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1398,7 +1316,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>18</v>
@@ -1409,7 +1327,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>19</v>
@@ -1420,7 +1338,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>20</v>
@@ -1431,7 +1349,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>21</v>
@@ -1442,7 +1360,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>22</v>
@@ -1453,7 +1371,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>23</v>
@@ -1464,7 +1382,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>24</v>
@@ -1475,7 +1393,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>25</v>
@@ -1486,7 +1404,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="B10">
         <v>26</v>
@@ -1497,7 +1415,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>27</v>
@@ -1508,7 +1426,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B12">
         <v>28</v>
@@ -1519,7 +1437,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B13">
         <v>29</v>
@@ -1530,7 +1448,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B14">
         <v>30</v>
@@ -1541,7 +1459,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B15">
         <v>31</v>
@@ -1552,7 +1470,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="B16">
         <v>32</v>
@@ -1563,7 +1481,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B17">
         <v>33</v>
@@ -1574,7 +1492,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="B18">
         <v>34</v>
@@ -1585,7 +1503,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B19">
         <v>35</v>
@@ -1596,7 +1514,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B20">
         <v>36</v>
@@ -1607,7 +1525,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B21">
         <v>37</v>
@@ -1618,7 +1536,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="B22">
         <v>38</v>
@@ -1629,7 +1547,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B23">
         <v>39</v>
@@ -1640,7 +1558,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="B24">
         <v>40</v>
@@ -1651,7 +1569,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B25">
         <v>41</v>
@@ -1662,7 +1580,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B26">
         <v>42</v>
@@ -1673,7 +1591,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B27">
         <v>43</v>
@@ -1684,7 +1602,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B28">
         <v>44</v>
@@ -1695,7 +1613,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B29">
         <v>45</v>
@@ -1706,7 +1624,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B30">
         <v>46</v>
@@ -1717,7 +1635,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B31">
         <v>47</v>
@@ -1728,7 +1646,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B32">
         <v>48</v>
@@ -1739,7 +1657,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="B33">
         <v>49</v>
@@ -1750,7 +1668,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B34">
         <v>50</v>
@@ -1761,7 +1679,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B35" t="s">
         <v>89</v>
@@ -1772,7 +1690,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
         <v>5</v>
@@ -1795,7 +1713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -2162,10 +2080,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2198,6 +2116,22 @@
         <v>46</v>
       </c>
     </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Add spread sheets for the new code tables.
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/AnalyticsCodeTables.xlsx
+++ b/booking-jail/r-load/AnalyticsCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="663" firstSheet="7" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="663" firstSheet="11" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="YesNo" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,11 @@
     <sheet name="Jurisdiction" sheetId="20" r:id="rId13"/>
     <sheet name="PopulationType" sheetId="22" r:id="rId14"/>
     <sheet name="PretrialStatus" sheetId="23" r:id="rId15"/>
+    <sheet name="HousingStatus" sheetId="26" r:id="rId16"/>
+    <sheet name="IncomeLevel" sheetId="27" r:id="rId17"/>
+    <sheet name="Occupation" sheetId="28" r:id="rId18"/>
+    <sheet name="Education" sheetId="29" r:id="rId19"/>
+    <sheet name="Language" sheetId="30" r:id="rId20"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="167">
   <si>
     <t>Yes</t>
   </si>
@@ -318,6 +323,222 @@
   </si>
   <si>
     <t>Deposit</t>
+  </si>
+  <si>
+    <t>HousingStatusID</t>
+  </si>
+  <si>
+    <t>HousingStatusDescription</t>
+  </si>
+  <si>
+    <t>Housing Status 1</t>
+  </si>
+  <si>
+    <t>Housing Status 2</t>
+  </si>
+  <si>
+    <t>Housing Status 3</t>
+  </si>
+  <si>
+    <t>Housing Status 4</t>
+  </si>
+  <si>
+    <t>Housing Status 5</t>
+  </si>
+  <si>
+    <t>Housing Status 6</t>
+  </si>
+  <si>
+    <t>Housing Status 7</t>
+  </si>
+  <si>
+    <t>IncomeLevelID</t>
+  </si>
+  <si>
+    <t>IncomeLevel</t>
+  </si>
+  <si>
+    <t>OccupationID</t>
+  </si>
+  <si>
+    <t>Occupation</t>
+  </si>
+  <si>
+    <t>EducationID</t>
+  </si>
+  <si>
+    <t>EducationLevel</t>
+  </si>
+  <si>
+    <t>8th grade or less</t>
+  </si>
+  <si>
+    <t>Some high school</t>
+  </si>
+  <si>
+    <t>GED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High school diploma </t>
+  </si>
+  <si>
+    <t>Some college</t>
+  </si>
+  <si>
+    <t xml:space="preserve">College graduate or more </t>
+  </si>
+  <si>
+    <t>Occupation 1</t>
+  </si>
+  <si>
+    <t>Occupation 2</t>
+  </si>
+  <si>
+    <t>Occupation 3</t>
+  </si>
+  <si>
+    <t>Occupation 4</t>
+  </si>
+  <si>
+    <t>Occupation 5</t>
+  </si>
+  <si>
+    <t>Occupation 6</t>
+  </si>
+  <si>
+    <t>Occupation 7</t>
+  </si>
+  <si>
+    <t>Occupation 8</t>
+  </si>
+  <si>
+    <t>Occupation 9</t>
+  </si>
+  <si>
+    <t>Occupation 10</t>
+  </si>
+  <si>
+    <t>Occupation 11</t>
+  </si>
+  <si>
+    <t>Occupation 12</t>
+  </si>
+  <si>
+    <t>LanguageID</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>Tagalog</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>Vietnamese</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>Korean</t>
+  </si>
+  <si>
+    <t>Russian</t>
+  </si>
+  <si>
+    <t>Arabic</t>
+  </si>
+  <si>
+    <t>Italian</t>
+  </si>
+  <si>
+    <t>Portuguese</t>
+  </si>
+  <si>
+    <t>Hungarian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polish </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hindi </t>
+  </si>
+  <si>
+    <t>ASL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Japanese </t>
+  </si>
+  <si>
+    <t>Persian</t>
+  </si>
+  <si>
+    <t>Urdu</t>
+  </si>
+  <si>
+    <t>Gujarati</t>
+  </si>
+  <si>
+    <t>Greek</t>
+  </si>
+  <si>
+    <t>Serbo-Croatian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Punjabi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Armenian </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hebrew </t>
+  </si>
+  <si>
+    <t>Cambodian</t>
+  </si>
+  <si>
+    <t>Hmong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navajo </t>
+  </si>
+  <si>
+    <t>Thai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yiddish </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laotian </t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Less than $300 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">$300-599 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">$600-999 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">$1,000-1,999 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">$2,000 or more </t>
   </si>
 </sst>
 </file>
@@ -1084,7 +1305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1139,6 +1360,380 @@
       </c>
       <c r="B6" t="s">
         <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1232,6 +1827,282 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
@@ -1293,7 +2164,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Correct the typo in agency names.
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/AnalyticsCodeTables.xlsx
+++ b/booking-jail/r-load/AnalyticsCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="663" firstSheet="11" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="663" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="YesNo" sheetId="1" r:id="rId1"/>
@@ -100,36 +100,6 @@
     <t>AgencyName</t>
   </si>
   <si>
-    <t>Agenty 1</t>
-  </si>
-  <si>
-    <t>Agenty 2</t>
-  </si>
-  <si>
-    <t>Agenty 3</t>
-  </si>
-  <si>
-    <t>Agenty 4</t>
-  </si>
-  <si>
-    <t>Agenty 5</t>
-  </si>
-  <si>
-    <t>Agenty 6</t>
-  </si>
-  <si>
-    <t>Agenty 7</t>
-  </si>
-  <si>
-    <t>Agenty 8</t>
-  </si>
-  <si>
-    <t>Agenty 9</t>
-  </si>
-  <si>
-    <t>Agenty 10</t>
-  </si>
-  <si>
     <t>BedTypeID</t>
   </si>
   <si>
@@ -539,6 +509,36 @@
   </si>
   <si>
     <t xml:space="preserve">$2,000 or more </t>
+  </si>
+  <si>
+    <t>Agency 1</t>
+  </si>
+  <si>
+    <t>Agency 2</t>
+  </si>
+  <si>
+    <t>Agency 3</t>
+  </si>
+  <si>
+    <t>Agency 4</t>
+  </si>
+  <si>
+    <t>Agency 5</t>
+  </si>
+  <si>
+    <t>Agency 6</t>
+  </si>
+  <si>
+    <t>Agency 7</t>
+  </si>
+  <si>
+    <t>Agency 8</t>
+  </si>
+  <si>
+    <t>Agency 9</t>
+  </si>
+  <si>
+    <t>Agency 10</t>
   </si>
 </sst>
 </file>
@@ -602,9 +602,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -979,10 +980,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -990,7 +991,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -998,7 +999,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1006,7 +1007,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1014,7 +1015,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1022,7 +1023,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1051,10 +1052,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1062,7 +1063,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1070,7 +1071,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1078,7 +1079,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1086,7 +1087,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1094,7 +1095,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1102,7 +1103,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1120,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1132,13 +1133,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1146,9 +1147,9 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2">
+        <v>55</v>
+      </c>
+      <c r="C2" s="2">
         <v>5000</v>
       </c>
     </row>
@@ -1157,9 +1158,9 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3">
+        <v>56</v>
+      </c>
+      <c r="C3" s="2">
         <v>1000</v>
       </c>
     </row>
@@ -1189,10 +1190,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1200,7 +1201,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1208,7 +1209,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1216,7 +1217,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1224,7 +1225,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1232,7 +1233,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1240,7 +1241,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1269,10 +1270,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1280,7 +1281,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1288,7 +1289,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1316,10 +1317,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1327,7 +1328,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1335,7 +1336,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1343,7 +1344,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1351,7 +1352,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1359,7 +1360,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1388,10 +1389,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1399,7 +1400,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1407,7 +1408,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1415,7 +1416,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1423,7 +1424,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1431,7 +1432,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1439,7 +1440,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1447,7 +1448,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1464,7 +1465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -1476,10 +1477,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1487,7 +1488,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1495,7 +1496,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1503,7 +1504,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1511,7 +1512,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1519,7 +1520,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1527,7 +1528,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1555,10 +1556,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1566,7 +1567,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1574,7 +1575,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1582,7 +1583,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1590,7 +1591,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1598,7 +1599,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1606,7 +1607,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1614,7 +1615,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1622,7 +1623,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1630,7 +1631,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1638,7 +1639,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1646,7 +1647,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1654,7 +1655,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1682,10 +1683,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1693,7 +1694,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1701,7 +1702,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1709,7 +1710,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1717,7 +1718,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1725,7 +1726,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1733,7 +1734,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1805,7 +1806,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1839,10 +1840,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1850,7 +1851,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1858,7 +1859,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1866,7 +1867,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1874,7 +1875,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1882,7 +1883,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1890,7 +1891,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1898,7 +1899,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1906,7 +1907,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1914,7 +1915,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1922,7 +1923,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1930,7 +1931,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1938,7 +1939,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1946,7 +1947,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1954,7 +1955,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1962,7 +1963,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1970,7 +1971,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1978,7 +1979,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1986,7 +1987,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1994,7 +1995,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -2002,7 +2003,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -2010,7 +2011,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -2018,7 +2019,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -2026,7 +2027,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -2034,7 +2035,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -2042,7 +2043,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -2050,7 +2051,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -2058,7 +2059,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -2066,7 +2067,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -2074,7 +2075,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -2082,7 +2083,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -2090,7 +2091,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2553,7 +2554,7 @@
         <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C35">
         <v>6</v>
@@ -2599,10 +2600,10 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2610,10 +2611,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2621,10 +2622,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2632,10 +2633,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2643,10 +2644,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2654,10 +2655,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2665,10 +2666,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2697,7 +2698,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2718,7 +2719,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2726,7 +2727,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2734,7 +2735,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2742,7 +2743,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2750,7 +2751,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2758,7 +2759,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2766,7 +2767,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2774,7 +2775,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2782,7 +2783,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2790,7 +2791,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2828,10 +2829,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2839,7 +2840,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2847,7 +2848,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2855,7 +2856,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2863,7 +2864,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2892,10 +2893,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2903,7 +2904,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2911,7 +2912,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2919,7 +2920,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2927,7 +2928,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2935,7 +2936,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2965,10 +2966,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2976,7 +2977,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2984,7 +2985,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2992,7 +2993,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3000,7 +3001,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove the YesNo code table.
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/AnalyticsCodeTables.xlsx
+++ b/booking-jail/r-load/AnalyticsCodeTables.xlsx
@@ -4,29 +4,28 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="663" firstSheet="3" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="663"/>
   </bookViews>
   <sheets>
-    <sheet name="YesNo" sheetId="1" r:id="rId1"/>
-    <sheet name="PersonRace" sheetId="2" r:id="rId2"/>
-    <sheet name="PersonSex" sheetId="3" r:id="rId3"/>
-    <sheet name="PersonAge" sheetId="4" r:id="rId4"/>
-    <sheet name="PersonAgeRange" sheetId="25" r:id="rId5"/>
-    <sheet name="Agency" sheetId="9" r:id="rId6"/>
-    <sheet name="BedType" sheetId="12" r:id="rId7"/>
-    <sheet name="BehaviorHealthType" sheetId="13" r:id="rId8"/>
-    <sheet name="BondType" sheetId="14" r:id="rId9"/>
-    <sheet name="CaseStatus" sheetId="17" r:id="rId10"/>
-    <sheet name="ChargeType" sheetId="18" r:id="rId11"/>
-    <sheet name="Facility" sheetId="19" r:id="rId12"/>
-    <sheet name="Jurisdiction" sheetId="20" r:id="rId13"/>
-    <sheet name="PopulationType" sheetId="22" r:id="rId14"/>
-    <sheet name="PretrialStatus" sheetId="23" r:id="rId15"/>
-    <sheet name="HousingStatus" sheetId="26" r:id="rId16"/>
-    <sheet name="IncomeLevel" sheetId="27" r:id="rId17"/>
-    <sheet name="Occupation" sheetId="28" r:id="rId18"/>
-    <sheet name="Education" sheetId="29" r:id="rId19"/>
-    <sheet name="Language" sheetId="30" r:id="rId20"/>
+    <sheet name="PersonRace" sheetId="2" r:id="rId1"/>
+    <sheet name="PersonSex" sheetId="3" r:id="rId2"/>
+    <sheet name="PersonAge" sheetId="4" r:id="rId3"/>
+    <sheet name="PersonAgeRange" sheetId="25" r:id="rId4"/>
+    <sheet name="Agency" sheetId="9" r:id="rId5"/>
+    <sheet name="BedType" sheetId="12" r:id="rId6"/>
+    <sheet name="BehaviorHealthType" sheetId="13" r:id="rId7"/>
+    <sheet name="BondType" sheetId="14" r:id="rId8"/>
+    <sheet name="CaseStatus" sheetId="17" r:id="rId9"/>
+    <sheet name="ChargeType" sheetId="18" r:id="rId10"/>
+    <sheet name="Facility" sheetId="19" r:id="rId11"/>
+    <sheet name="Jurisdiction" sheetId="20" r:id="rId12"/>
+    <sheet name="PopulationType" sheetId="22" r:id="rId13"/>
+    <sheet name="PretrialStatus" sheetId="23" r:id="rId14"/>
+    <sheet name="HousingStatus" sheetId="26" r:id="rId15"/>
+    <sheet name="IncomeLevel" sheetId="27" r:id="rId16"/>
+    <sheet name="Occupation" sheetId="28" r:id="rId17"/>
+    <sheet name="Education" sheetId="29" r:id="rId18"/>
+    <sheet name="Language" sheetId="30" r:id="rId19"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -38,13 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="167">
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="163">
   <si>
     <t>Asian</t>
   </si>
@@ -86,12 +79,6 @@
   </si>
   <si>
     <t>PersonRaceDescription</t>
-  </si>
-  <si>
-    <t>YesNoID</t>
-  </si>
-  <si>
-    <t>YesNoDescription</t>
   </si>
   <si>
     <t>AgencyID</t>
@@ -919,23 +906,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="33.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -951,11 +939,44 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -965,78 +986,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD58"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="73.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -1052,10 +1001,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1063,7 +1012,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1071,7 +1020,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1079,7 +1028,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1087,7 +1036,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1095,7 +1044,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1103,7 +1052,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1117,11 +1066,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
@@ -1133,13 +1082,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1147,7 +1096,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C2" s="2">
         <v>5000</v>
@@ -1158,7 +1107,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C3" s="2">
         <v>1000</v>
@@ -1174,7 +1123,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -1190,10 +1139,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1201,7 +1150,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1209,7 +1158,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1217,7 +1166,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1225,7 +1174,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1233,7 +1182,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1241,7 +1190,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1254,7 +1203,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1270,10 +1219,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1281,7 +1230,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1289,7 +1238,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1302,7 +1251,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1317,10 +1266,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1328,7 +1277,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1336,7 +1285,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1344,7 +1293,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1352,7 +1301,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1360,7 +1309,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1373,7 +1322,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -1389,10 +1338,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1400,7 +1349,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1408,7 +1357,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1416,7 +1365,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1424,7 +1373,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1432,7 +1381,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1440,7 +1389,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1448,7 +1397,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1461,7 +1410,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -1477,10 +1426,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1488,7 +1437,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1496,7 +1445,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1504,7 +1453,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1512,7 +1461,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1520,7 +1469,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1528,7 +1477,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1541,7 +1490,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -1556,10 +1505,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1567,7 +1516,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1575,7 +1524,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1583,7 +1532,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1591,7 +1540,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1599,7 +1548,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1607,7 +1556,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1615,7 +1564,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1623,7 +1572,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1631,7 +1580,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1639,7 +1588,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1647,7 +1596,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1655,7 +1604,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1668,7 +1617,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -1683,10 +1632,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1694,7 +1643,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1702,7 +1651,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1710,7 +1659,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1718,7 +1667,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1726,7 +1675,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1734,7 +1683,283 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1748,363 +1973,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>150</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -2120,10 +1988,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2131,7 +1999,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2139,7 +2007,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2147,7 +2015,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2160,7 +2028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
@@ -2177,13 +2045,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2554,7 +2422,7 @@
         <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C35">
         <v>6</v>
@@ -2565,7 +2433,7 @@
         <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C36">
         <v>7</v>
@@ -2581,7 +2449,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -2597,13 +2465,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2611,10 +2479,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2622,10 +2490,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2633,10 +2501,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2644,10 +2512,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2655,10 +2523,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2666,10 +2534,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2677,10 +2545,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2693,7 +2561,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -2708,10 +2576,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2719,7 +2587,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2727,7 +2595,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2735,7 +2603,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2743,7 +2611,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2751,7 +2619,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2759,7 +2627,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2767,7 +2635,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2775,7 +2643,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2783,7 +2651,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2791,7 +2659,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2799,7 +2667,7 @@
         <v>999</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2813,7 +2681,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -2829,10 +2697,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2840,7 +2708,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2848,7 +2716,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2856,7 +2724,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2864,7 +2732,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -2877,7 +2745,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -2893,10 +2761,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2904,7 +2772,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2912,7 +2780,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2920,7 +2788,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2928,7 +2796,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2936,7 +2804,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2950,7 +2818,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -2966,10 +2834,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2977,7 +2845,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2985,7 +2853,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2993,7 +2861,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3001,7 +2869,79 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="73.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove Facility table and dimension, rename BehaviorHealth to BehavioralHealth.
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/AnalyticsCodeTables.xlsx
+++ b/booking-jail/r-load/AnalyticsCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="663"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="663" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="PersonRace" sheetId="2" r:id="rId1"/>
@@ -13,19 +13,18 @@
     <sheet name="PersonAgeRange" sheetId="25" r:id="rId4"/>
     <sheet name="Agency" sheetId="9" r:id="rId5"/>
     <sheet name="BedType" sheetId="12" r:id="rId6"/>
-    <sheet name="BehaviorHealthType" sheetId="13" r:id="rId7"/>
+    <sheet name="BehavioralHealthType" sheetId="13" r:id="rId7"/>
     <sheet name="BondType" sheetId="14" r:id="rId8"/>
     <sheet name="CaseStatus" sheetId="17" r:id="rId9"/>
     <sheet name="ChargeType" sheetId="18" r:id="rId10"/>
-    <sheet name="Facility" sheetId="19" r:id="rId11"/>
-    <sheet name="Jurisdiction" sheetId="20" r:id="rId12"/>
-    <sheet name="PopulationType" sheetId="22" r:id="rId13"/>
-    <sheet name="PretrialStatus" sheetId="23" r:id="rId14"/>
-    <sheet name="HousingStatus" sheetId="26" r:id="rId15"/>
-    <sheet name="IncomeLevel" sheetId="27" r:id="rId16"/>
-    <sheet name="Occupation" sheetId="28" r:id="rId17"/>
-    <sheet name="Education" sheetId="29" r:id="rId18"/>
-    <sheet name="Language" sheetId="30" r:id="rId19"/>
+    <sheet name="Jurisdiction" sheetId="20" r:id="rId11"/>
+    <sheet name="PopulationType" sheetId="22" r:id="rId12"/>
+    <sheet name="PretrialStatus" sheetId="23" r:id="rId13"/>
+    <sheet name="HousingStatus" sheetId="26" r:id="rId14"/>
+    <sheet name="IncomeLevel" sheetId="27" r:id="rId15"/>
+    <sheet name="Occupation" sheetId="28" r:id="rId16"/>
+    <sheet name="Education" sheetId="29" r:id="rId17"/>
+    <sheet name="Language" sheetId="30" r:id="rId18"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="158">
   <si>
     <t>Asian</t>
   </si>
@@ -105,12 +104,6 @@
     <t>BedType 4</t>
   </si>
   <si>
-    <t>BehaviorHealthTypeID</t>
-  </si>
-  <si>
-    <t>BehaviorHealthDescription</t>
-  </si>
-  <si>
     <t>Disorder 1</t>
   </si>
   <si>
@@ -183,21 +176,6 @@
     <t>Charge 6</t>
   </si>
   <si>
-    <t>FacilityID</t>
-  </si>
-  <si>
-    <t>FacilityName</t>
-  </si>
-  <si>
-    <t>Capacity</t>
-  </si>
-  <si>
-    <t>Facility 1</t>
-  </si>
-  <si>
-    <t>Facility 2</t>
-  </si>
-  <si>
     <t>JurisdictionID</t>
   </si>
   <si>
@@ -526,6 +504,12 @@
   </si>
   <si>
     <t>Agency 10</t>
+  </si>
+  <si>
+    <t>BehavioralHealthTypeID</t>
+  </si>
+  <si>
+    <t>BehavioralHealthDescription</t>
   </si>
 </sst>
 </file>
@@ -589,10 +573,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -908,7 +891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -963,7 +946,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1001,10 +984,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1012,7 +995,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1020,7 +1003,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1028,7 +1011,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1036,7 +1019,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1044,7 +1027,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1052,7 +1035,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1067,63 +1050,6 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="2" max="2" width="37.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="2">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -1139,10 +1065,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1150,7 +1076,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1158,7 +1084,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1166,7 +1092,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1174,7 +1100,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1182,7 +1108,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1190,7 +1116,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1203,7 +1129,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1219,10 +1145,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1230,7 +1156,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1238,7 +1164,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1251,7 +1177,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1266,10 +1192,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1277,7 +1203,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1285,7 +1211,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1293,7 +1219,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1301,7 +1227,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1309,7 +1235,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1322,7 +1248,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -1338,10 +1264,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1349,7 +1275,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1357,7 +1283,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1365,7 +1291,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1373,7 +1299,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1381,7 +1307,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1389,7 +1315,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1397,7 +1323,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1410,7 +1336,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -1426,10 +1352,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1437,7 +1363,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1445,7 +1371,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1453,7 +1379,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1461,7 +1387,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1469,7 +1395,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1477,7 +1403,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1490,7 +1416,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -1505,10 +1431,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1516,7 +1442,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1524,7 +1450,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1532,7 +1458,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1540,7 +1466,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1548,7 +1474,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1556,7 +1482,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1564,7 +1490,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1572,7 +1498,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1580,7 +1506,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1588,7 +1514,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1596,7 +1522,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1604,7 +1530,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1617,7 +1543,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -1632,10 +1558,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1643,7 +1569,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1651,7 +1577,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1659,7 +1585,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1667,7 +1593,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1675,7 +1601,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1683,7 +1609,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1696,7 +1622,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B32"/>
   <sheetViews>
@@ -1708,10 +1634,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1719,7 +1645,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1727,7 +1653,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1735,7 +1661,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1743,7 +1669,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1751,7 +1677,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1759,7 +1685,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1767,7 +1693,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1775,7 +1701,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1783,7 +1709,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1791,7 +1717,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1799,7 +1725,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1807,7 +1733,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1815,7 +1741,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1823,7 +1749,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1831,7 +1757,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1839,7 +1765,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1847,7 +1773,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1855,7 +1781,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1863,7 +1789,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1871,7 +1797,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1879,7 +1805,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1887,7 +1813,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1895,7 +1821,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1903,7 +1829,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1911,7 +1837,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1919,7 +1845,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1927,7 +1853,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1935,7 +1861,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1943,7 +1869,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1951,7 +1877,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1959,7 +1885,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2422,7 +2348,7 @@
         <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C35">
         <v>6</v>
@@ -2468,10 +2394,10 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2479,10 +2405,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2490,10 +2416,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2501,10 +2427,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2512,10 +2438,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2523,10 +2449,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2534,10 +2460,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2587,7 +2513,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2595,7 +2521,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2603,7 +2529,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2611,7 +2537,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2619,7 +2545,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2627,7 +2553,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2635,7 +2561,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2643,7 +2569,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2651,7 +2577,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2659,7 +2585,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2749,8 +2675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2761,10 +2687,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2772,7 +2698,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2780,7 +2706,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2788,7 +2714,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2796,7 +2722,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2804,7 +2730,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2834,10 +2760,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2845,7 +2771,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2853,7 +2779,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2861,7 +2787,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2869,7 +2795,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2898,10 +2824,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2909,7 +2835,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2917,7 +2843,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2925,7 +2851,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2933,7 +2859,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2941,7 +2867,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename the code tables and column names to go with naming convention. The Agency and Jurisdition tables are not renamed.
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/AnalyticsCodeTables.xlsx
+++ b/booking-jail/r-load/AnalyticsCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="663" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="663" firstSheet="11" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="PersonRace" sheetId="2" r:id="rId1"/>
@@ -15,16 +15,16 @@
     <sheet name="BedType" sheetId="12" r:id="rId6"/>
     <sheet name="BehavioralHealthType" sheetId="13" r:id="rId7"/>
     <sheet name="BondType" sheetId="14" r:id="rId8"/>
-    <sheet name="CaseStatus" sheetId="17" r:id="rId9"/>
+    <sheet name="CaseStatusType" sheetId="17" r:id="rId9"/>
     <sheet name="ChargeType" sheetId="18" r:id="rId10"/>
     <sheet name="Jurisdiction" sheetId="20" r:id="rId11"/>
     <sheet name="PopulationType" sheetId="22" r:id="rId12"/>
-    <sheet name="PretrialStatus" sheetId="23" r:id="rId13"/>
-    <sheet name="HousingStatus" sheetId="26" r:id="rId14"/>
-    <sheet name="IncomeLevel" sheetId="27" r:id="rId15"/>
-    <sheet name="Occupation" sheetId="28" r:id="rId16"/>
-    <sheet name="Education" sheetId="29" r:id="rId17"/>
-    <sheet name="Language" sheetId="30" r:id="rId18"/>
+    <sheet name="PretrialStatusType" sheetId="23" r:id="rId13"/>
+    <sheet name="HousingStatusType" sheetId="26" r:id="rId14"/>
+    <sheet name="IncomeLevelType" sheetId="27" r:id="rId15"/>
+    <sheet name="OccupationType" sheetId="28" r:id="rId16"/>
+    <sheet name="EducationType" sheetId="29" r:id="rId17"/>
+    <sheet name="LanguageType" sheetId="30" r:id="rId18"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -89,9 +89,6 @@
     <t>BedTypeID</t>
   </si>
   <si>
-    <t>BedType</t>
-  </si>
-  <si>
     <t>BedType 1</t>
   </si>
   <si>
@@ -122,21 +119,12 @@
     <t>BondTypeID</t>
   </si>
   <si>
-    <t>BondType</t>
-  </si>
-  <si>
     <t>Cash</t>
   </si>
   <si>
     <t>Surety</t>
   </si>
   <si>
-    <t>StatusID</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Status 1</t>
   </si>
   <si>
@@ -155,9 +143,6 @@
     <t>ChargeTypeID</t>
   </si>
   <si>
-    <t>ChargeType</t>
-  </si>
-  <si>
     <t>Charge 1</t>
   </si>
   <si>
@@ -203,21 +188,12 @@
     <t>PopulationTypeID</t>
   </si>
   <si>
-    <t>PopulationType</t>
-  </si>
-  <si>
     <t>Normal</t>
   </si>
   <si>
     <t>Target</t>
   </si>
   <si>
-    <t>PretrialStatus</t>
-  </si>
-  <si>
-    <t>PretrialStatusID</t>
-  </si>
-  <si>
     <t>Jail</t>
   </si>
   <si>
@@ -260,12 +236,6 @@
     <t>Deposit</t>
   </si>
   <si>
-    <t>HousingStatusID</t>
-  </si>
-  <si>
-    <t>HousingStatusDescription</t>
-  </si>
-  <si>
     <t>Housing Status 1</t>
   </si>
   <si>
@@ -287,21 +257,6 @@
     <t>Housing Status 7</t>
   </si>
   <si>
-    <t>IncomeLevelID</t>
-  </si>
-  <si>
-    <t>IncomeLevel</t>
-  </si>
-  <si>
-    <t>OccupationID</t>
-  </si>
-  <si>
-    <t>Occupation</t>
-  </si>
-  <si>
-    <t>EducationID</t>
-  </si>
-  <si>
     <t>EducationLevel</t>
   </si>
   <si>
@@ -359,12 +314,6 @@
     <t>Occupation 12</t>
   </si>
   <si>
-    <t>LanguageID</t>
-  </si>
-  <si>
-    <t>Language</t>
-  </si>
-  <si>
     <t>English</t>
   </si>
   <si>
@@ -510,6 +459,57 @@
   </si>
   <si>
     <t>BehavioralHealthDescription</t>
+  </si>
+  <si>
+    <t>BedTypeDescription</t>
+  </si>
+  <si>
+    <t>BondTypeDescription</t>
+  </si>
+  <si>
+    <t>CaseStatusTypeID</t>
+  </si>
+  <si>
+    <t>CaseStatusTypeDescription</t>
+  </si>
+  <si>
+    <t>ChargeTypeDescription</t>
+  </si>
+  <si>
+    <t>PopulationTypeDescription</t>
+  </si>
+  <si>
+    <t>HousingStatusTypeID</t>
+  </si>
+  <si>
+    <t>HousingStatusTypeDescription</t>
+  </si>
+  <si>
+    <t>IncomeLevelTypeID</t>
+  </si>
+  <si>
+    <t>IncomeLevelTypeDescription</t>
+  </si>
+  <si>
+    <t>OccupationTypeID</t>
+  </si>
+  <si>
+    <t>OccupationTypeDescription</t>
+  </si>
+  <si>
+    <t>EducationTypeID</t>
+  </si>
+  <si>
+    <t>LanguageTypeID</t>
+  </si>
+  <si>
+    <t>LanguageTypeDescription</t>
+  </si>
+  <si>
+    <t>PretrialStatusTypeID</t>
+  </si>
+  <si>
+    <t>PretrialStatusTypeDescription</t>
   </si>
 </sst>
 </file>
@@ -946,7 +946,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -973,7 +973,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -984,10 +984,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -995,7 +995,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1003,7 +1003,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1011,7 +1011,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1019,7 +1019,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1027,7 +1027,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1035,7 +1035,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1065,10 +1065,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1076,7 +1076,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1084,7 +1084,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1092,7 +1092,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1100,7 +1100,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1108,7 +1108,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1116,7 +1116,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1134,21 +1134,21 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1156,7 +1156,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1164,7 +1164,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1182,20 +1182,21 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>156</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1203,7 +1204,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1211,7 +1212,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1219,7 +1220,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1227,7 +1228,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1235,7 +1236,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1253,21 +1254,21 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>147</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1275,7 +1276,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1283,7 +1284,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1291,7 +1292,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1299,7 +1300,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1307,7 +1308,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1315,7 +1316,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1323,7 +1324,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1340,22 +1341,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>149</v>
       </c>
       <c r="B1" t="s">
-        <v>84</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1363,7 +1364,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1371,7 +1372,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1379,7 +1380,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1387,7 +1388,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1395,7 +1396,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1403,7 +1404,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1421,20 +1422,20 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>151</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1442,7 +1443,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1450,7 +1451,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1458,7 +1459,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1466,7 +1467,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1474,7 +1475,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1482,7 +1483,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1490,7 +1491,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1498,7 +1499,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1506,7 +1507,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1514,7 +1515,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1522,7 +1523,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1530,7 +1531,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1548,20 +1549,21 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>153</v>
       </c>
       <c r="B1" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1569,7 +1571,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1577,7 +1579,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1585,7 +1587,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1593,7 +1595,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1601,7 +1603,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1609,7 +1611,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1627,17 +1629,21 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>107</v>
+        <v>154</v>
       </c>
       <c r="B1" t="s">
-        <v>108</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1645,7 +1651,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1653,7 +1659,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1661,7 +1667,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1669,7 +1675,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1677,7 +1683,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1685,7 +1691,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1693,7 +1699,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1701,7 +1707,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1709,7 +1715,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1717,7 +1723,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1725,7 +1731,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1733,7 +1739,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1741,7 +1747,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1749,7 +1755,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1757,7 +1763,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1765,7 +1771,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1773,7 +1779,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1781,7 +1787,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1789,7 +1795,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1797,7 +1803,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1805,7 +1811,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1813,7 +1819,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1821,7 +1827,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1829,7 +1835,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1837,7 +1843,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1845,7 +1851,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1853,7 +1859,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1861,7 +1867,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1869,7 +1875,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1877,7 +1883,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1885,7 +1891,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2348,7 +2354,7 @@
         <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C35">
         <v>6</v>
@@ -2394,10 +2400,10 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2405,10 +2411,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2416,10 +2422,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2427,10 +2433,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2438,10 +2444,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2449,10 +2455,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2460,10 +2466,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2513,7 +2519,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2521,7 +2527,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2529,7 +2535,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2537,7 +2543,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2545,7 +2551,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2553,7 +2559,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2561,7 +2567,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2569,7 +2575,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2577,7 +2583,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2585,7 +2591,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2611,8 +2617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView topLeftCell="A239" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2626,7 +2632,7 @@
         <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2634,7 +2640,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2642,7 +2648,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2650,7 +2656,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2658,7 +2664,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2675,22 +2681,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="B1" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2698,7 +2704,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2706,7 +2712,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2714,7 +2720,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2722,7 +2728,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2730,7 +2736,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2749,7 +2755,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2760,10 +2766,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2771,7 +2777,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2779,7 +2785,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2787,7 +2793,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2795,7 +2801,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2813,7 +2819,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD58"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2824,10 +2830,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2835,7 +2841,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2843,7 +2849,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2851,7 +2857,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2859,7 +2865,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2867,7 +2873,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename Agency, Jurisdiction and EducationType tables.
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/AnalyticsCodeTables.xlsx
+++ b/booking-jail/r-load/AnalyticsCodeTables.xlsx
@@ -4,26 +4,26 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="663" firstSheet="11" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="663" firstSheet="11" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="PersonRace" sheetId="2" r:id="rId1"/>
     <sheet name="PersonSex" sheetId="3" r:id="rId2"/>
     <sheet name="PersonAge" sheetId="4" r:id="rId3"/>
     <sheet name="PersonAgeRange" sheetId="25" r:id="rId4"/>
-    <sheet name="Agency" sheetId="9" r:id="rId5"/>
+    <sheet name="AgencyType" sheetId="9" r:id="rId5"/>
     <sheet name="BedType" sheetId="12" r:id="rId6"/>
     <sheet name="BehavioralHealthType" sheetId="13" r:id="rId7"/>
     <sheet name="BondType" sheetId="14" r:id="rId8"/>
     <sheet name="CaseStatusType" sheetId="17" r:id="rId9"/>
     <sheet name="ChargeType" sheetId="18" r:id="rId10"/>
-    <sheet name="Jurisdiction" sheetId="20" r:id="rId11"/>
+    <sheet name="JurisdictionType" sheetId="20" r:id="rId11"/>
     <sheet name="PopulationType" sheetId="22" r:id="rId12"/>
     <sheet name="PretrialStatusType" sheetId="23" r:id="rId13"/>
     <sheet name="HousingStatusType" sheetId="26" r:id="rId14"/>
     <sheet name="IncomeLevelType" sheetId="27" r:id="rId15"/>
     <sheet name="OccupationType" sheetId="28" r:id="rId16"/>
-    <sheet name="EducationType" sheetId="29" r:id="rId17"/>
+    <sheet name="EducationLevelType" sheetId="29" r:id="rId17"/>
     <sheet name="LanguageType" sheetId="30" r:id="rId18"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -80,12 +80,6 @@
     <t>PersonRaceDescription</t>
   </si>
   <si>
-    <t>AgencyID</t>
-  </si>
-  <si>
-    <t>AgencyName</t>
-  </si>
-  <si>
     <t>BedTypeID</t>
   </si>
   <si>
@@ -161,12 +155,6 @@
     <t>Charge 6</t>
   </si>
   <si>
-    <t>JurisdictionID</t>
-  </si>
-  <si>
-    <t>JurisdictionName</t>
-  </si>
-  <si>
     <t>Jurisdiction 1</t>
   </si>
   <si>
@@ -257,9 +245,6 @@
     <t>Housing Status 7</t>
   </si>
   <si>
-    <t>EducationLevel</t>
-  </si>
-  <si>
     <t>8th grade or less</t>
   </si>
   <si>
@@ -497,9 +482,6 @@
     <t>OccupationTypeDescription</t>
   </si>
   <si>
-    <t>EducationTypeID</t>
-  </si>
-  <si>
     <t>LanguageTypeID</t>
   </si>
   <si>
@@ -510,6 +492,24 @@
   </si>
   <si>
     <t>PretrialStatusTypeDescription</t>
+  </si>
+  <si>
+    <t>AgencyTypeID</t>
+  </si>
+  <si>
+    <t>AgencyTypeDescription</t>
+  </si>
+  <si>
+    <t>JurisdictionTypeID</t>
+  </si>
+  <si>
+    <t>JurisdictionTypeDescription</t>
+  </si>
+  <si>
+    <t>EducationLevelTypeID</t>
+  </si>
+  <si>
+    <t>EducationLevelTypeDescription</t>
   </si>
 </sst>
 </file>
@@ -946,7 +946,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -984,10 +984,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -995,7 +995,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1003,7 +1003,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1011,7 +1011,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1019,7 +1019,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1027,7 +1027,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1035,7 +1035,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1053,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1065,10 +1065,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>154</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1076,7 +1076,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1084,7 +1084,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1092,7 +1092,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1100,7 +1100,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1108,7 +1108,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1116,7 +1116,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1145,10 +1145,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1156,7 +1156,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1164,7 +1164,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1193,10 +1193,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1204,7 +1204,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1212,7 +1212,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1220,7 +1220,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1228,7 +1228,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1236,7 +1236,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1265,10 +1265,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1276,7 +1276,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1284,7 +1284,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1292,7 +1292,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1300,7 +1300,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1308,7 +1308,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1316,7 +1316,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1324,7 +1324,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1341,7 +1341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -1353,10 +1353,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1364,7 +1364,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1372,7 +1372,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1380,7 +1380,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1388,7 +1388,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1396,7 +1396,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1404,7 +1404,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1432,10 +1432,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1443,7 +1443,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1451,7 +1451,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1459,7 +1459,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1467,7 +1467,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1475,7 +1475,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1483,7 +1483,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1491,7 +1491,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1499,7 +1499,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1507,7 +1507,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1515,7 +1515,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1523,7 +1523,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1531,7 +1531,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1548,22 +1548,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1571,7 +1571,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1579,7 +1579,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1587,7 +1587,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1595,7 +1595,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1603,7 +1603,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1611,7 +1611,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1640,10 +1640,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1651,7 +1651,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1659,7 +1659,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1667,7 +1667,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1675,7 +1675,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1683,7 +1683,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1691,7 +1691,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1699,7 +1699,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1707,7 +1707,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1715,7 +1715,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1723,7 +1723,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1731,7 +1731,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1739,7 +1739,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1747,7 +1747,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1755,7 +1755,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1763,7 +1763,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1771,7 +1771,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1779,7 +1779,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1787,7 +1787,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1795,7 +1795,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1803,7 +1803,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1811,7 +1811,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1819,7 +1819,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1827,7 +1827,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1835,7 +1835,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1843,7 +1843,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1851,7 +1851,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1859,7 +1859,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1867,7 +1867,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1875,7 +1875,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1883,7 +1883,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1891,7 +1891,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2354,7 +2354,7 @@
         <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C35">
         <v>6</v>
@@ -2400,10 +2400,10 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2411,10 +2411,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2422,10 +2422,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2433,10 +2433,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2444,10 +2444,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2455,10 +2455,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2466,10 +2466,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2498,20 +2498,21 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>152</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2519,7 +2520,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2527,7 +2528,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2535,7 +2536,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2543,7 +2544,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2551,7 +2552,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2559,7 +2560,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2567,7 +2568,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2575,7 +2576,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2583,7 +2584,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2591,7 +2592,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2629,10 +2630,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2640,7 +2641,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2648,7 +2649,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2656,7 +2657,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2664,7 +2665,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2693,10 +2694,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2704,7 +2705,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2712,7 +2713,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2720,7 +2721,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2728,7 +2729,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2736,7 +2737,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2766,10 +2767,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2777,7 +2778,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2785,7 +2786,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2793,7 +2794,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2801,7 +2802,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2830,10 +2831,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2841,7 +2842,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2849,7 +2850,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2857,7 +2858,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2865,7 +2866,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2873,7 +2874,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates with some values provided by AC
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/AnalyticsCodeTables.xlsx
+++ b/booking-jail/r-load/AnalyticsCodeTables.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="663" firstSheet="11" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="15675" tabRatio="663" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PersonRace" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="118">
   <si>
     <t>Asian</t>
   </si>
@@ -137,51 +137,9 @@
     <t>ChargeTypeID</t>
   </si>
   <si>
-    <t>Charge 1</t>
-  </si>
-  <si>
-    <t>Charge 2</t>
-  </si>
-  <si>
-    <t>Charge 3</t>
-  </si>
-  <si>
-    <t>Charge 4</t>
-  </si>
-  <si>
-    <t>Charge 5</t>
-  </si>
-  <si>
-    <t>Charge 6</t>
-  </si>
-  <si>
-    <t>Jurisdiction 1</t>
-  </si>
-  <si>
-    <t>Jurisdiction 2</t>
-  </si>
-  <si>
-    <t>Jurisdiction 3</t>
-  </si>
-  <si>
-    <t>Jurisdiction 4</t>
-  </si>
-  <si>
-    <t>Jurisdiction 5</t>
-  </si>
-  <si>
-    <t>Jurisdiction 6</t>
-  </si>
-  <si>
     <t>PopulationTypeID</t>
   </si>
   <si>
-    <t>Normal</t>
-  </si>
-  <si>
-    <t>Target</t>
-  </si>
-  <si>
     <t>Jail</t>
   </si>
   <si>
@@ -245,24 +203,6 @@
     <t>Housing Status 7</t>
   </si>
   <si>
-    <t>8th grade or less</t>
-  </si>
-  <si>
-    <t>Some high school</t>
-  </si>
-  <si>
-    <t>GED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High school diploma </t>
-  </si>
-  <si>
-    <t>Some college</t>
-  </si>
-  <si>
-    <t xml:space="preserve">College graduate or more </t>
-  </si>
-  <si>
     <t>Occupation 1</t>
   </si>
   <si>
@@ -299,147 +239,6 @@
     <t>Occupation 12</t>
   </si>
   <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>Spanish</t>
-  </si>
-  <si>
-    <t>Chinese</t>
-  </si>
-  <si>
-    <t>Tagalog</t>
-  </si>
-  <si>
-    <t>French</t>
-  </si>
-  <si>
-    <t>Vietnamese</t>
-  </si>
-  <si>
-    <t>German</t>
-  </si>
-  <si>
-    <t>Korean</t>
-  </si>
-  <si>
-    <t>Russian</t>
-  </si>
-  <si>
-    <t>Arabic</t>
-  </si>
-  <si>
-    <t>Italian</t>
-  </si>
-  <si>
-    <t>Portuguese</t>
-  </si>
-  <si>
-    <t>Hungarian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Polish </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hindi </t>
-  </si>
-  <si>
-    <t>ASL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Japanese </t>
-  </si>
-  <si>
-    <t>Persian</t>
-  </si>
-  <si>
-    <t>Urdu</t>
-  </si>
-  <si>
-    <t>Gujarati</t>
-  </si>
-  <si>
-    <t>Greek</t>
-  </si>
-  <si>
-    <t>Serbo-Croatian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Punjabi </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Armenian </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hebrew </t>
-  </si>
-  <si>
-    <t>Cambodian</t>
-  </si>
-  <si>
-    <t>Hmong</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Navajo </t>
-  </si>
-  <si>
-    <t>Thai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yiddish </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laotian </t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Less than $300 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">$300-599 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">$600-999 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">$1,000-1,999 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">$2,000 or more </t>
-  </si>
-  <si>
-    <t>Agency 1</t>
-  </si>
-  <si>
-    <t>Agency 2</t>
-  </si>
-  <si>
-    <t>Agency 3</t>
-  </si>
-  <si>
-    <t>Agency 4</t>
-  </si>
-  <si>
-    <t>Agency 5</t>
-  </si>
-  <si>
-    <t>Agency 6</t>
-  </si>
-  <si>
-    <t>Agency 7</t>
-  </si>
-  <si>
-    <t>Agency 8</t>
-  </si>
-  <si>
-    <t>Agency 9</t>
-  </si>
-  <si>
-    <t>Agency 10</t>
-  </si>
-  <si>
     <t>BehavioralHealthTypeID</t>
   </si>
   <si>
@@ -510,6 +309,87 @@
   </si>
   <si>
     <t>EducationLevelTypeDescription</t>
+  </si>
+  <si>
+    <t>Adams County SO</t>
+  </si>
+  <si>
+    <t>Arvada PD</t>
+  </si>
+  <si>
+    <t>Aurora PD</t>
+  </si>
+  <si>
+    <t>Brighton PD</t>
+  </si>
+  <si>
+    <t>Commerce City PD</t>
+  </si>
+  <si>
+    <t>Federal Heights PD</t>
+  </si>
+  <si>
+    <t>Northglenn PD</t>
+  </si>
+  <si>
+    <t>Thornton PD</t>
+  </si>
+  <si>
+    <t>Westminster PD</t>
+  </si>
+  <si>
+    <t>State Court</t>
+  </si>
+  <si>
+    <t>County Court</t>
+  </si>
+  <si>
+    <t>Municipal Court</t>
+  </si>
+  <si>
+    <t>General Population</t>
+  </si>
+  <si>
+    <t>Target Population</t>
+  </si>
+  <si>
+    <t>Felony</t>
+  </si>
+  <si>
+    <t>Misdemeanor</t>
+  </si>
+  <si>
+    <t>Municipal</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Level 1</t>
+  </si>
+  <si>
+    <t>Level 2</t>
+  </si>
+  <si>
+    <t>Level 3</t>
+  </si>
+  <si>
+    <t>Level 4</t>
+  </si>
+  <si>
+    <t>Level 5</t>
+  </si>
+  <si>
+    <t>Level 6</t>
+  </si>
+  <si>
+    <t>Language 1</t>
+  </si>
+  <si>
+    <t>Language 2</t>
+  </si>
+  <si>
+    <t>Language 3</t>
   </si>
 </sst>
 </file>
@@ -895,13 +775,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -909,7 +789,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -917,7 +797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -925,7 +805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -933,7 +813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -941,15 +821,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -970,72 +850,64 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1051,72 +923,56 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A6" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
-    <col min="2" max="2" width="29.83203125" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>154</v>
+        <v>87</v>
       </c>
       <c r="B1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1131,40 +987,48 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1185,37 +1049,37 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>150</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1223,7 +1087,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1231,12 +1095,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1257,74 +1121,74 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1339,72 +1203,80 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>144</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1419,119 +1291,135 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>79</v>
       </c>
       <c r="B1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>86</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>98</v>
+      </c>
+      <c r="B14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>99</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1546,72 +1434,88 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>89</v>
       </c>
       <c r="B1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1626,272 +1530,64 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>148</v>
+        <v>81</v>
       </c>
       <c r="B1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>117</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1912,13 +1608,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1926,7 +1622,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1934,7 +1630,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1942,7 +1638,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1968,14 +1664,14 @@
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" customWidth="1"/>
-    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1986,7 +1682,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>18</v>
       </c>
@@ -1997,7 +1693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>19</v>
       </c>
@@ -2008,7 +1704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20</v>
       </c>
@@ -2019,7 +1715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>21</v>
       </c>
@@ -2030,7 +1726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>22</v>
       </c>
@@ -2041,7 +1737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>23</v>
       </c>
@@ -2052,7 +1748,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>24</v>
       </c>
@@ -2063,7 +1759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>25</v>
       </c>
@@ -2074,7 +1770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>26</v>
       </c>
@@ -2085,7 +1781,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>27</v>
       </c>
@@ -2096,7 +1792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>28</v>
       </c>
@@ -2107,7 +1803,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>29</v>
       </c>
@@ -2118,7 +1814,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>30</v>
       </c>
@@ -2129,7 +1825,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>31</v>
       </c>
@@ -2140,7 +1836,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>32</v>
       </c>
@@ -2151,7 +1847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>33</v>
       </c>
@@ -2162,7 +1858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>34</v>
       </c>
@@ -2173,7 +1869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>35</v>
       </c>
@@ -2184,7 +1880,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>36</v>
       </c>
@@ -2195,7 +1891,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>37</v>
       </c>
@@ -2206,7 +1902,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>38</v>
       </c>
@@ -2217,7 +1913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>39</v>
       </c>
@@ -2228,7 +1924,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>40</v>
       </c>
@@ -2239,7 +1935,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>41</v>
       </c>
@@ -2250,7 +1946,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>42</v>
       </c>
@@ -2261,7 +1957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>43</v>
       </c>
@@ -2272,7 +1968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>44</v>
       </c>
@@ -2283,7 +1979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>45</v>
       </c>
@@ -2294,7 +1990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>46</v>
       </c>
@@ -2305,7 +2001,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>47</v>
       </c>
@@ -2316,7 +2012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>48</v>
       </c>
@@ -2327,7 +2023,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>49</v>
       </c>
@@ -2338,7 +2034,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>50</v>
       </c>
@@ -2349,18 +2045,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C35">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>52</v>
       </c>
@@ -2385,94 +2081,94 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2495,111 +2191,103 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>152</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
-        <v>999</v>
-      </c>
-      <c r="B12" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2622,21 +2310,21 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" customWidth="1"/>
-    <col min="2" max="2" width="39.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2644,7 +2332,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2652,7 +2340,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2660,7 +2348,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2686,21 +2374,21 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>134</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2708,7 +2396,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2716,7 +2404,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2724,7 +2412,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2732,7 +2420,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2759,21 +2447,21 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="34.5" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2781,7 +2469,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2789,20 +2477,20 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2823,21 +2511,21 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="73.5" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="73.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>138</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2845,7 +2533,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2853,7 +2541,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2861,7 +2549,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2869,7 +2557,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Update demo load for booking/jail to use more realistic code lists
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/AnalyticsCodeTables.xlsx
+++ b/booking-jail/r-load/AnalyticsCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="15675" tabRatio="663" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="15675" tabRatio="663" firstSheet="4" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="PersonRace" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="117">
   <si>
     <t>Asian</t>
   </si>
@@ -345,9 +345,6 @@
   </si>
   <si>
     <t>Municipal Court</t>
-  </si>
-  <si>
-    <t>General Population</t>
   </si>
   <si>
     <t>Target Population</t>
@@ -875,7 +872,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -883,7 +880,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -891,7 +888,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -899,7 +896,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -989,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,10 +1014,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1228,7 +1225,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1236,7 +1233,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1244,7 +1241,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1252,7 +1249,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1260,7 +1257,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1268,7 +1265,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1411,7 +1408,7 @@
         <v>98</v>
       </c>
       <c r="B14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1459,7 +1456,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1467,7 +1464,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1475,7 +1472,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1483,7 +1480,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1491,7 +1488,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1499,7 +1496,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1507,7 +1504,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1555,7 +1552,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1563,7 +1560,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1571,7 +1568,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1579,7 +1576,7 @@
         <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2081,7 +2078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update pretrial status code table per Debbie's direction (change jail to "no bond" and make it less likely to occur)
</commit_message>
<xml_diff>
--- a/booking-jail/r-load/AnalyticsCodeTables.xlsx
+++ b/booking-jail/r-load/AnalyticsCodeTables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="15675" tabRatio="663" firstSheet="4" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="15675" tabRatio="663" firstSheet="4" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="PersonRace" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="EducationLevelType" sheetId="29" r:id="rId17"/>
     <sheet name="LanguageType" sheetId="30" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -140,9 +140,6 @@
     <t>PopulationTypeID</t>
   </si>
   <si>
-    <t>Jail</t>
-  </si>
-  <si>
     <t>SRP</t>
   </si>
   <si>
@@ -387,6 +384,9 @@
   </si>
   <si>
     <t>Language 3</t>
+  </si>
+  <si>
+    <t>No Bond</t>
   </si>
 </sst>
 </file>
@@ -823,7 +823,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -864,7 +864,7 @@
         <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -872,7 +872,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -880,7 +880,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -888,7 +888,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -896,7 +896,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -934,10 +934,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s">
         <v>87</v>
-      </c>
-      <c r="B1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -945,7 +945,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -953,7 +953,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -961,7 +961,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -986,7 +986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1001,7 +1001,7 @@
         <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1009,7 +1009,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1017,7 +1017,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1042,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,10 +1054,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
         <v>83</v>
-      </c>
-      <c r="B1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1065,7 +1065,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1073,7 +1073,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1097,7 +1097,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1126,10 +1126,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
         <v>75</v>
-      </c>
-      <c r="B1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1137,7 +1137,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1145,7 +1145,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1153,7 +1153,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1161,7 +1161,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1169,7 +1169,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1177,7 +1177,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1185,7 +1185,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1214,10 +1214,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
         <v>77</v>
-      </c>
-      <c r="B1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1225,7 +1225,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1233,7 +1233,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1241,7 +1241,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1249,7 +1249,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1257,7 +1257,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1265,7 +1265,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1301,10 +1301,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
         <v>79</v>
-      </c>
-      <c r="B1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1312,7 +1312,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1320,7 +1320,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1328,7 +1328,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1336,7 +1336,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1344,7 +1344,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1352,7 +1352,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1360,7 +1360,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1368,7 +1368,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1376,7 +1376,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1384,7 +1384,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1392,7 +1392,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1400,7 +1400,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1408,7 +1408,7 @@
         <v>98</v>
       </c>
       <c r="B14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1445,10 +1445,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
         <v>89</v>
-      </c>
-      <c r="B1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1456,7 +1456,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1464,7 +1464,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1472,7 +1472,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1480,7 +1480,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1488,7 +1488,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1496,7 +1496,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1504,7 +1504,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1541,10 +1541,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
         <v>81</v>
-      </c>
-      <c r="B1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1552,7 +1552,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1560,7 +1560,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1568,7 +1568,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1576,7 +1576,7 @@
         <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2047,7 +2047,7 @@
         <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C35">
         <v>6</v>
@@ -2093,10 +2093,10 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
         <v>43</v>
-      </c>
-      <c r="C1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2104,10 +2104,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2115,10 +2115,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2126,10 +2126,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2137,10 +2137,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2148,10 +2148,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2159,10 +2159,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2202,10 +2202,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" t="s">
         <v>85</v>
-      </c>
-      <c r="B1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2213,7 +2213,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2221,7 +2221,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2229,7 +2229,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2237,7 +2237,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2245,7 +2245,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2253,7 +2253,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2261,7 +2261,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2269,7 +2269,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2277,7 +2277,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2318,7 +2318,7 @@
         <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2379,10 +2379,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
         <v>67</v>
-      </c>
-      <c r="B1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2455,7 +2455,7 @@
         <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2479,7 +2479,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2487,7 +2487,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2516,10 +2516,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
         <v>71</v>
-      </c>
-      <c r="B1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>